<commit_message>
- Added ToDataSet and ToDataTable extensions, - Added some extensions for ExcelWorksheet object, - Added and updated test, - and incremented minor version
</commit_message>
<xml_diff>
--- a/test/EPPlus.Core.Extensions.Tests/Resources/testsheets.xlsx
+++ b/test/EPPlus.Core.Extensions.Tests/Resources/testsheets.xlsx
@@ -5,24 +5,25 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Workspace\_trendyol\EpPlus.Core.Extensions\test\EPPlus.Core.Extensions.Tests\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aydin.eraydin\Desktop\EPPlus.Core.Extensions\test\EPPlus.Core.Extensions.Tests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TEST1" sheetId="1" r:id="rId1"/>
     <sheet name="TEST2" sheetId="2" r:id="rId2"/>
     <sheet name="TEST3" sheetId="3" r:id="rId3"/>
     <sheet name="TEST4" sheetId="4" r:id="rId4"/>
+    <sheet name="TEST5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913" calcOnSave="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -155,11 +156,20 @@
   <si>
     <t>barcode324</t>
   </si>
+  <si>
+    <t>Barcode2</t>
+  </si>
+  <si>
+    <t>Barcode1</t>
+  </si>
+  <si>
+    <t>Barcode3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0\ [$USD]"/>
   </numFmts>
@@ -289,8 +299,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TEST4" displayName="TEST4" ref="A1:C5" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:C5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TEST4" displayName="TEST4" ref="F9:H13" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="F9:H13"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Barcode"/>
     <tableColumn id="2" name="Quantity"/>
@@ -935,10 +945,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="F9:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,55 +958,55 @@
     <col min="3" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="9" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="10" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="1">
+      <c r="H10" s="1">
         <v>42964</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="11" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
         <v>39</v>
       </c>
-      <c r="B3" t="s">
+      <c r="G11" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="12" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
         <v>42</v>
       </c>
-      <c r="B4">
+      <c r="G12">
         <v>3</v>
       </c>
-      <c r="C4" s="1">
+      <c r="H12" s="1">
         <v>42964.470081018517</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="13" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
         <v>43</v>
       </c>
-      <c r="B5">
+      <c r="G13">
         <v>55</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="H13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1004,4 +1014,67 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1">
+        <v>42955</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1">
+        <v>42955</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>42955</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- Added AsEnumerable<T>() and ToList<T>() extension methods for ExcelWorksheet, - Bug fixes and consolidations, - Incremented version
</commit_message>
<xml_diff>
--- a/test/EPPlus.Core.Extensions.Tests/Resources/testsheets.xlsx
+++ b/test/EPPlus.Core.Extensions.Tests/Resources/testsheets.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aydin.eraydin\Desktop\EPPlus.Core.Extensions\test\EPPlus.Core.Extensions.Tests\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aydin.eraydin\Desktop\x\EPPlus.Core.Extensions\test\EPPlus.Core.Extensions.Tests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TEST1" sheetId="1" r:id="rId1"/>
@@ -299,8 +299,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TEST4" displayName="TEST4" ref="F9:H13" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="F9:H13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TEST4" displayName="TEST4" ref="E9:G13" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="E9:G13"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Barcode"/>
     <tableColumn id="2" name="Quantity"/>
@@ -945,68 +945,63 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F9:H13"/>
+  <dimension ref="E9:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="9" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="F9" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F10" t="s">
+    <row r="10" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="1">
+      <c r="G10" s="1">
         <v>42964</v>
       </c>
     </row>
-    <row r="11" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
       <c r="F11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
+    <row r="12" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
         <v>42</v>
       </c>
-      <c r="G12">
+      <c r="F12">
         <v>3</v>
       </c>
-      <c r="H12" s="1">
+      <c r="G12" s="1">
         <v>42964.470081018517</v>
       </c>
     </row>
-    <row r="13" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F13" t="s">
+    <row r="13" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
         <v>43</v>
       </c>
-      <c r="G13">
+      <c r="F13">
         <v>55</v>
       </c>
-      <c r="H13" s="1"/>
+      <c r="G13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1020,7 +1015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Implemented new methods on ExcelPackage class, and renamed some methods
</commit_message>
<xml_diff>
--- a/test/EPPlus.Core.Extensions.Tests/Resources/testsheets.xlsx
+++ b/test/EPPlus.Core.Extensions.Tests/Resources/testsheets.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aydin.eraydin\Desktop\x\EPPlus.Core.Extensions\test\EPPlus.Core.Extensions.Tests\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aydin.eraydin\Desktop\repos\EPPlus.Core.Extensions\test\EPPlus.Core.Extensions.Tests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TEST1" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="TEST3" sheetId="3" r:id="rId3"/>
     <sheet name="TEST4" sheetId="4" r:id="rId4"/>
     <sheet name="TEST5" sheetId="5" r:id="rId5"/>
+    <sheet name="TEST6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913" calcOnSave="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -947,11 +948,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E9:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="9" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E9" s="3" t="s">
@@ -1016,7 +1021,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,4 +1077,58 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1">
+        <v>42955</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1">
+        <v>42955</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- Added DeleteColum(headerText) method for ExcelWorksheet object, - Added  BorderAround(style), SetBorderColor(color), BorderAround(style, color) methods for ExcelRangeBase object - And, some consolidations.
</commit_message>
<xml_diff>
--- a/test/EPPlus.Core.Extensions.Tests/Resources/testsheets.xlsx
+++ b/test/EPPlus.Core.Extensions.Tests/Resources/testsheets.xlsx
@@ -949,7 +949,7 @@
   <dimension ref="E9:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:G13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,15 +1081,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>35</v>
       </c>
@@ -1099,8 +1099,11 @@
       <c r="C1" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -1110,8 +1113,10 @@
       <c r="C2" s="1">
         <v>42955</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1121,12 +1126,16 @@
       <c r="C3" s="1">
         <v>42955</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>46</v>
       </c>
       <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed custom formatted datetime parse problem
</commit_message>
<xml_diff>
--- a/test/EPPlus.Core.Extensions.Tests/Resources/testsheets.xlsx
+++ b/test/EPPlus.Core.Extensions.Tests/Resources/testsheets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aydin.eraydin\Desktop\repos\EPPlus.Core.Extensions\test\EPPlus.Core.Extensions.Tests\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aydin.eraydin\Desktop\repos\ExcelOperations\EPPlus.Core.Extensions\test\EPPlus.Core.Extensions.Tests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
     <sheet name="TEST5" sheetId="5" r:id="rId5"/>
     <sheet name="TEST6" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -171,8 +171,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0\ [$USD]"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -213,11 +215,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1084,10 +1089,13 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -1096,7 +1104,7 @@
       <c r="B1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D1" s="3"/>
@@ -1110,7 +1118,7 @@
       <c r="B2">
         <v>23</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="5">
         <v>42955</v>
       </c>
       <c r="D2" s="1"/>
@@ -1123,8 +1131,8 @@
       <c r="B3">
         <v>12</v>
       </c>
-      <c r="C3" s="1">
-        <v>42955</v>
+      <c r="C3" s="6">
+        <v>42677.063113425924</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1133,11 +1141,11 @@
       <c r="A4" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated packages, and fixed a bug inside GetColumns()
</commit_message>
<xml_diff>
--- a/test/EPPlus.Core.Extensions.Tests/Resources/testsheets.xlsx
+++ b/test/EPPlus.Core.Extensions.Tests/Resources/testsheets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aydin.eraydin\Desktop\repos\ExcelOperations\EPPlus.Core.Extensions\test\EPPlus.Core.Extensions.Tests\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Workspace\EPPlus.Core.Extensions\test\EPPlus.Core.Extensions.Tests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1086,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A2:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1097,52 +1097,52 @@
     <col min="3" max="3" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2">
-        <v>23</v>
-      </c>
-      <c r="C2" s="5">
-        <v>42955</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B3">
-        <v>12</v>
-      </c>
-      <c r="C3" s="6">
-        <v>42677.063113425924</v>
+        <v>23</v>
+      </c>
+      <c r="C3" s="5">
+        <v>42955</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4" s="6">
+        <v>42677.063113425924</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed some known issues
</commit_message>
<xml_diff>
--- a/test/EPPlus.Core.Extensions.Tests/Resources/testsheets.xlsx
+++ b/test/EPPlus.Core.Extensions.Tests/Resources/testsheets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20112" windowHeight="8016" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="TEST1" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="TEST4" sheetId="4" r:id="rId4"/>
     <sheet name="TEST5" sheetId="5" r:id="rId5"/>
     <sheet name="TEST6" sheetId="6" r:id="rId6"/>
+    <sheet name="TEST7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -609,14 +610,14 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="4" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="3" max="4" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -633,7 +634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -650,7 +651,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -667,7 +668,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -684,7 +685,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -701,7 +702,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -731,16 +732,16 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -748,7 +749,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -756,7 +757,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -764,19 +765,19 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -801,16 +802,16 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>29</v>
       </c>
@@ -830,7 +831,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>22</v>
       </c>
@@ -850,7 +851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>19</v>
       </c>
@@ -870,7 +871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>20</v>
       </c>
@@ -890,7 +891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>18</v>
       </c>
@@ -907,7 +908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>21</v>
       </c>
@@ -924,7 +925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>34</v>
       </c>
@@ -957,13 +958,13 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E9" s="3" t="s">
         <v>35</v>
       </c>
@@ -974,7 +975,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E10" t="s">
         <v>38</v>
       </c>
@@ -982,7 +983,7 @@
         <v>42964</v>
       </c>
     </row>
-    <row r="11" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
         <v>39</v>
       </c>
@@ -993,7 +994,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
         <v>42</v>
       </c>
@@ -1004,7 +1005,7 @@
         <v>42964.470081018517</v>
       </c>
     </row>
-    <row r="13" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
         <v>43</v>
       </c>
@@ -1029,12 +1030,12 @@
       <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>35</v>
       </c>
@@ -1045,7 +1046,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -1056,7 +1057,7 @@
         <v>42955</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1067,7 +1068,7 @@
         <v>42955</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1088,16 +1089,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
@@ -1111,7 +1112,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1124,7 +1125,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1137,7 +1138,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1148,4 +1149,30 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- Fixed null exception problem which occured while converting empty worksheet to list of objects. - Version incremented (v2.0.0)
</commit_message>
<xml_diff>
--- a/test/EPPlus.Core.Extensions.Tests/Resources/testsheets.xlsx
+++ b/test/EPPlus.Core.Extensions.Tests/Resources/testsheets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20112" windowHeight="8016" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="TEST1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="TEST5" sheetId="5" r:id="rId5"/>
     <sheet name="TEST6" sheetId="6" r:id="rId6"/>
     <sheet name="TEST7" sheetId="7" r:id="rId7"/>
+    <sheet name="EmptySheet" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -610,14 +611,14 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="3" max="4" width="9.88671875" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="4" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -634,7 +635,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -651,7 +652,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -668,7 +669,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -685,7 +686,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -702,7 +703,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -735,13 +736,13 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.109375" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -749,7 +750,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -757,7 +758,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -765,19 +766,19 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -802,16 +803,16 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.5546875" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="27.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>29</v>
       </c>
@@ -831,7 +832,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>22</v>
       </c>
@@ -851,7 +852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>19</v>
       </c>
@@ -871,7 +872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>20</v>
       </c>
@@ -891,7 +892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>18</v>
       </c>
@@ -908,7 +909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>21</v>
       </c>
@@ -925,7 +926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>34</v>
       </c>
@@ -958,13 +959,13 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E9" s="3" t="s">
         <v>35</v>
       </c>
@@ -975,7 +976,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>38</v>
       </c>
@@ -983,7 +984,7 @@
         <v>42964</v>
       </c>
     </row>
-    <row r="11" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>39</v>
       </c>
@@ -994,7 +995,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>42</v>
       </c>
@@ -1005,7 +1006,7 @@
         <v>42964.470081018517</v>
       </c>
     </row>
-    <row r="13" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>43</v>
       </c>
@@ -1030,12 +1031,12 @@
       <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>35</v>
       </c>
@@ -1046,7 +1047,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -1057,7 +1058,7 @@
         <v>42955</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1068,7 +1069,7 @@
         <v>42955</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1093,12 +1094,12 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
@@ -1112,7 +1113,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1125,7 +1126,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1138,7 +1139,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1155,13 +1156,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>35</v>
       </c>
@@ -1175,4 +1176,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>